<commit_message>
Fixed some unwanted lines
</commit_message>
<xml_diff>
--- a/packet_info.xlsx
+++ b/packet_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,22 +453,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>66.22.244.26</t>
+          <t>162.159.135.234</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>50003</v>
+        <v>443</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ether / IP / UDP 192.168.1.80:64182 &gt; 66.22.244.26:50003 / Raw</t>
+          <t>Ether / IP / TCP 192.168.1.80:52490 &gt; 162.159.135.234:https A</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>162.159.135.234</t>
+          <t>185.199.111.154</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -476,22 +476,37 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ether / IP / TCP 192.168.1.80:52490 &gt; 162.159.135.234:https A</t>
+          <t>Ether / IP / TCP 192.168.1.80:52821 &gt; 185.199.111.154:https A / Raw</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>66.22.244.25</t>
+          <t>185.199.111.154</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50021</v>
+        <v>443</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ether / IP / UDP 192.168.1.80:50431 &gt; 66.22.244.25:50021 / Raw</t>
+          <t>Ether / IP / TCP 192.168.1.80:52813 &gt; 185.199.111.154:https A / Raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>140.82.114.26</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>443</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ether / IP / TCP 192.168.1.80:52824 &gt; 140.82.114.26:https A / Raw</t>
         </is>
       </c>
     </row>

</xml_diff>